<commit_message>
Updated to version 1.7
</commit_message>
<xml_diff>
--- a/Latest Version/Assets/Data Log.xlsx
+++ b/Latest Version/Assets/Data Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12300" windowWidth="28800" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12300" windowWidth="28800" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Late" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
   <si>
     <t>Datetime</t>
   </si>
@@ -32,6 +32,18 @@
     <t>TESTING5</t>
   </si>
   <si>
+    <t>13/10/2018 22:41</t>
+  </si>
+  <si>
+    <t>T0121212Y</t>
+  </si>
+  <si>
+    <t>13/10/2018 22:45</t>
+  </si>
+  <si>
+    <t>TESTING1</t>
+  </si>
+  <si>
     <t>13/10/2018 10:58</t>
   </si>
   <si>
@@ -41,9 +53,6 @@
     <t>TESTING2</t>
   </si>
   <si>
-    <t>TESTING1</t>
-  </si>
-  <si>
     <t>TESTING6</t>
   </si>
   <si>
@@ -69,6 +78,12 @@
   </si>
   <si>
     <t>23</t>
+  </si>
+  <si>
+    <t>13/10/2018 22:39</t>
+  </si>
+  <si>
+    <t>31/10/2018 20:23</t>
   </si>
 </sst>
 </file>
@@ -396,8 +411,8 @@
   </sheetPr>
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
@@ -431,13 +446,28 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="2" t="n"/>
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="2" t="n"/>
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="2" t="n"/>
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="n"/>
@@ -543,7 +573,7 @@
   </sheetPr>
   <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -563,7 +593,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -571,15 +601,15 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -587,7 +617,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -595,15 +625,15 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -611,7 +641,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -619,42 +649,42 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -662,7 +692,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -670,7 +700,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -678,7 +708,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -686,7 +716,7 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -698,10 +728,20 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="2" t="n"/>
+      <c r="A19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="2" t="n"/>
+      <c r="A20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2" t="n"/>

</xml_diff>

<commit_message>
Updated to version 1.10"
</commit_message>
<xml_diff>
--- a/Latest Version/Assets/Data Log.xlsx
+++ b/Latest Version/Assets/Data Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jotham\Documents\Git Repos\Earlyve-System\Latest Version\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157B0625-D485-4C38-9F49-36E60F26C840}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1413A7-59CE-4770-A4AA-31863C187977}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
     <t>3D</t>
   </si>
   <si>
-    <t>stupid</t>
+    <t>MRT Breakdown</t>
   </si>
 </sst>
 </file>
@@ -555,7 +555,7 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>